<commit_message>
Added Contacts through API
</commit_message>
<xml_diff>
--- a/client/public/uploads/test.xlsx
+++ b/client/public/uploads/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hackathon Projects\flipr\client\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2A02A5-096E-496D-8CBC-D68F36C218CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064166FB-58B9-4C92-91BF-2B1B4E52C8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{C79EDA29-349B-486C-9E26-EA6D3EA55736}"/>
   </bookViews>
@@ -25,42 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Curran</t>
-  </si>
-  <si>
-    <t>sc@gmail.com</t>
-  </si>
-  <si>
-    <t>vk@gmail.com</t>
-  </si>
-  <si>
-    <t>rs@gmail.com</t>
-  </si>
-  <si>
-    <t>Virat</t>
-  </si>
-  <si>
-    <t>kohli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohit </t>
-  </si>
-  <si>
-    <t>Sharma</t>
   </si>
   <si>
     <t>LastName</t>
   </si>
   <si>
     <t>FirstName</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>def@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -423,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08886764-F18A-4DD4-B287-F2D4359AD4DA}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,50 +420,26 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{628EFBF5-C420-441D-93F3-E117F4BDC244}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{2AFA556B-9A38-4738-AD63-32BA7368C194}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{701683FE-805E-4FFA-8A44-9047054AA31F}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{19A05E8A-F19B-4260-A6DE-E6EF5B3BE33A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Weekly Monthyl and Yearly Mails
</commit_message>
<xml_diff>
--- a/client/public/uploads/test.xlsx
+++ b/client/public/uploads/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hackathon Projects\flipr\client\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064166FB-58B9-4C92-91BF-2B1B4E52C8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2A02A5-096E-496D-8CBC-D68F36C218CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{C79EDA29-349B-486C-9E26-EA6D3EA55736}"/>
   </bookViews>
@@ -25,21 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
   <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Curran</t>
+  </si>
+  <si>
+    <t>sc@gmail.com</t>
+  </si>
+  <si>
+    <t>vk@gmail.com</t>
+  </si>
+  <si>
+    <t>rs@gmail.com</t>
+  </si>
+  <si>
+    <t>Virat</t>
+  </si>
+  <si>
+    <t>kohli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohit </t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
     <t>LastName</t>
   </si>
   <si>
     <t>FirstName</t>
-  </si>
-  <si>
-    <t>def</t>
-  </si>
-  <si>
-    <t>def@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08886764-F18A-4DD4-B287-F2D4359AD4DA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,26 +441,50 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{19A05E8A-F19B-4260-A6DE-E6EF5B3BE33A}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{628EFBF5-C420-441D-93F3-E117F4BDC244}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{2AFA556B-9A38-4738-AD63-32BA7368C194}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{701683FE-805E-4FFA-8A44-9047054AA31F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>